<commit_message>
ajustado comentarios dos arquivos
</commit_message>
<xml_diff>
--- a/10-mergefullAB/merge.xlsx
+++ b/10-mergefullAB/merge.xlsx
@@ -522,7 +522,11 @@
           <t>Linha</t>
         </is>
       </c>
-      <c r="K7" s="2" t="inlineStr"/>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="13.8" r="8" s="3">
       <c r="A8" s="2" t="inlineStr"/>
@@ -584,7 +588,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J9" s="2" t="n"/>
+      <c r="J9" s="2" t="n">
+        <v>12</v>
+      </c>
       <c r="K9" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -630,7 +636,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J10" s="2" t="n"/>
+      <c r="J10" s="2" t="n">
+        <v>13</v>
+      </c>
       <c r="K10" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -676,7 +684,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J11" s="2" t="n"/>
+      <c r="J11" s="2" t="n">
+        <v>16</v>
+      </c>
       <c r="K11" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -722,7 +732,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J12" s="2" t="n"/>
+      <c r="J12" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -810,7 +822,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J15" s="2" t="n"/>
+      <c r="J15" s="2" t="n">
+        <v>18</v>
+      </c>
       <c r="K15" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -856,7 +870,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J16" s="2" t="n"/>
+      <c r="J16" s="2" t="n">
+        <v>19</v>
+      </c>
       <c r="K16" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -1238,7 +1254,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J33" s="2" t="n"/>
+      <c r="J33" s="2" t="n">
+        <v>24</v>
+      </c>
       <c r="K33" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -1325,7 +1343,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J36" s="2" t="n"/>
+      <c r="J36" s="2" t="n">
+        <v>8</v>
+      </c>
       <c r="K36" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -1371,7 +1391,9 @@
           <t>Comum</t>
         </is>
       </c>
-      <c r="J37" s="2" t="n"/>
+      <c r="J37" s="2" t="n">
+        <v>11</v>
+      </c>
       <c r="K37" s="2" t="inlineStr">
         <is>
           <t>Comum</t>
@@ -1388,7 +1410,7 @@
       <c r="G38" s="2" t="inlineStr"/>
       <c r="H38" s="2" t="inlineStr"/>
       <c r="I38" s="2" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="J38" s="2" t="inlineStr"/>
       <c r="K38" s="2" t="inlineStr"/>
     </row>
     <row r="39">

</xml_diff>